<commit_message>
Updated BOM with personal stash info
</commit_message>
<xml_diff>
--- a/hardware/manuf/BOM.xlsx
+++ b/hardware/manuf/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6890B80-C7E4-42ED-AAB8-326FAE8639D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39C69E1-88C5-486C-A757-AFF3F4B493B9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="121">
   <si>
     <t>IO Board:</t>
   </si>
@@ -371,6 +371,18 @@
   </si>
   <si>
     <t>POLARIZED CAPACITOR, European symbol</t>
+  </si>
+  <si>
+    <t>In Stash:</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>THONK</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -705,705 +717,768 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD27"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
       </c>
       <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>28</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>77</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>22</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
       </c>
       <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>33</v>
-      </c>
-      <c r="I8" t="s">
-        <v>34</v>
       </c>
       <c r="J8" t="s">
         <v>34</v>
       </c>
-      <c r="K8">
+      <c r="K8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
       </c>
       <c r="D9" t="s">
         <v>36</v>
       </c>
       <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
         <v>37</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>33</v>
-      </c>
-      <c r="I9" t="s">
-        <v>34</v>
       </c>
       <c r="J9" t="s">
         <v>34</v>
       </c>
-      <c r="K9">
+      <c r="K9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>44</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="U14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="V14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="W14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="Y14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Y14" s="1" t="s">
+      <c r="Z14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z14" s="1" t="s">
+      <c r="AA14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AA14" s="1" t="s">
+      <c r="AB14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AB14" s="1" t="s">
+      <c r="AC14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AC14" s="1" t="s">
+      <c r="AD14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AD14" s="1" t="s">
+      <c r="AE14" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15">
         <v>6</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>64</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>65</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>66</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>67</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>68</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>37</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>112</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>113</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>114</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>115</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>116</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Z16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17">
         <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>72</v>
       </c>
       <c r="C17" t="s">
         <v>72</v>
       </c>
       <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
         <v>73</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>74</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>75</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>76</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>77</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>78</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>72</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18">
         <v>5</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>79</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>80</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>81</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>82</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>83</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19">
         <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>92</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
       </c>
       <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" t="s">
         <v>93</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>94</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>95</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20">
         <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
       </c>
       <c r="C20" t="s">
         <v>98</v>
       </c>
       <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" t="s">
         <v>99</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>100</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>101</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>85</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>86</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>87</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>88</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>89</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" t="s">
         <v>90</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Y21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>102</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>103</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>104</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>105</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>106</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>107</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>108</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>109</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AA22" t="s">
         <v>110</v>
       </c>
-      <c r="AB22" t="s">
+      <c r="AC22" t="s">
         <v>111</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AD22" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>96</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>25</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>26</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>97</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>28</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>77</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24">
         <v>5</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>70</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>25</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>26</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>71</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>28</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>77</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25">
         <v>10</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>24</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>25</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>26</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>84</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>28</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>77</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Z25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>30</v>
-      </c>
-      <c r="C26" t="s">
-        <v>31</v>
       </c>
       <c r="D26" t="s">
         <v>31</v>
       </c>
       <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" t="s">
         <v>32</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>33</v>
-      </c>
-      <c r="O26" t="s">
-        <v>34</v>
       </c>
       <c r="P26" t="s">
         <v>34</v>
       </c>
-      <c r="T26">
+      <c r="Q26" t="s">
+        <v>34</v>
+      </c>
+      <c r="U26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
       </c>
       <c r="D27" t="s">
         <v>36</v>
       </c>
       <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" t="s">
         <v>37</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>33</v>
-      </c>
-      <c r="O27" t="s">
-        <v>34</v>
       </c>
       <c r="P27" t="s">
         <v>34</v>
       </c>
-      <c r="T27">
+      <c r="Q27" t="s">
+        <v>34</v>
+      </c>
+      <c r="U27">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A15:AD27">
-    <sortCondition ref="E15"/>
+  <sortState ref="B15:AE27">
+    <sortCondition ref="F15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>